<commit_message>
Added MS Jacdac connector and library
</commit_message>
<xml_diff>
--- a/Project Outputs for BlinkBoard_micro/BOM/Bill of Materials-BlinkBoard_micro.xlsx
+++ b/Project Outputs for BlinkBoard_micro/BOM/Bill of Materials-BlinkBoard_micro.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="173">
   <si>
     <t>Designator</t>
   </si>
@@ -92,10 +92,13 @@
     <t>J5</t>
   </si>
   <si>
-    <t>JACDAC_CONNECTOR</t>
-  </si>
-  <si>
-    <t/>
+    <t>Jacdac edge connector</t>
+  </si>
+  <si>
+    <t>3 pin Jacdac edge connector 1.27mm pitch</t>
+  </si>
+  <si>
+    <t>https://github.com/microsoft/jacdac-mdk/blob/main/connector/JACDAC-Connector-by-Yuliang-2020-11-28.pdf</t>
   </si>
   <si>
     <t>TP1, TP2</t>
@@ -1003,17 +1006,19 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+      <c r="L4" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1029,866 +1034,866 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H6" s="1">
         <v>0.14000000000000001</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J6" s="1">
         <v>1</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F7" s="1">
         <v>3</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H7" s="1">
         <v>0.17</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J7" s="1">
         <v>3</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H8" s="1">
         <v>0.1</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J8" s="1">
         <v>1</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H9" s="1">
         <v>0.11</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J9" s="1">
         <v>1</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H10" s="1">
         <v>0.23</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J10" s="1">
         <v>2</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H11" s="1">
         <v>0.22</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J11" s="1">
         <v>1</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="F12" s="1">
         <v>65</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H12" s="1">
         <v>29.95</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J12" s="1">
         <v>65</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H13" s="1">
         <v>0.18</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J13" s="1">
         <v>1</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="F14" s="1">
         <v>2</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H14" s="1">
         <v>0.28000000000000003</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J14" s="1">
         <v>2</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="F15" s="1">
         <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H15" s="1">
         <v>0.38</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J15" s="1">
         <v>1</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H16" s="1">
         <v>0.17</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J16" s="1">
         <v>1</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H17" s="1">
         <v>2.95</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J17" s="1">
         <v>1</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="F18" s="1">
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H18" s="1">
         <v>0.97</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J18" s="1">
         <v>1</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="F19" s="1">
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H19" s="1">
         <v>1.42</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J19" s="1">
         <v>1</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F20" s="1">
         <v>4</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H20" s="1">
         <v>0.1</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J20" s="1">
         <v>4</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F21" s="1">
         <v>2</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H21" s="1">
         <v>0.12</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J21" s="1">
         <v>2</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H22" s="1">
         <v>0.1</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J22" s="1">
         <v>1</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F23" s="1">
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H23" s="1">
         <v>0.1</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J23" s="1">
         <v>1</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H24" s="1">
         <v>0.4</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J24" s="1">
         <v>1</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H25" s="1">
         <v>0.1</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J25" s="1">
         <v>1</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="F26" s="1">
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H26" s="1">
         <v>0.76</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J26" s="1">
         <v>1</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="F27" s="1">
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H27" s="1">
         <v>1.72</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J27" s="1">
         <v>1</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="F28" s="1">
         <v>2</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H28" s="1">
         <v>0.39</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J28" s="1">
         <v>2</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="F29" s="1">
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H29" s="1">
         <v>3.08</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J29" s="1">
         <v>1</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>